<commit_message>
Added eval section, updated figures
</commit_message>
<xml_diff>
--- a/figs/results.xlsx
+++ b/figs/results.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="23540" tabRatio="500"/>
+    <workbookView xWindow="-36680" yWindow="680" windowWidth="38400" windowHeight="16920" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -19,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
   <si>
     <t>Read</t>
   </si>
@@ -39,16 +40,28 @@
     <t>B-W-C</t>
   </si>
   <si>
-    <t>WC</t>
-  </si>
-  <si>
     <t>Write</t>
   </si>
   <si>
     <t>B-R-W-C</t>
   </si>
   <si>
-    <t>BR-WC</t>
+    <t>BWC</t>
+  </si>
+  <si>
+    <t>BR-BWC</t>
+  </si>
+  <si>
+    <t>TX 1</t>
+  </si>
+  <si>
+    <t>TX 5</t>
+  </si>
+  <si>
+    <t>Omid 2</t>
+  </si>
+  <si>
+    <t>Lorra</t>
   </si>
 </sst>
 </file>
@@ -91,12 +104,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -108,18 +133,52 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="17">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -227,7 +286,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C0504D"/>
+              <a:srgbClr val="632523"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -278,6 +337,11 @@
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="008000"/>
+            </a:solidFill>
+          </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:dLbls>
             <c:delete val="1"/>
@@ -322,11 +386,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2117195896"/>
-        <c:axId val="-2117841992"/>
+        <c:axId val="-2132884136"/>
+        <c:axId val="-2133590664"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2117195896"/>
+        <c:axId val="-2132884136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -335,7 +399,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117841992"/>
+        <c:crossAx val="-2133590664"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -343,7 +407,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2117841992"/>
+        <c:axId val="-2133590664"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -374,7 +438,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2117195896"/>
+        <c:crossAx val="-2132884136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -449,7 +513,7 @@
                   <c:v>B-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>WC</c:v>
+                  <c:v>BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -501,7 +565,7 @@
                   <c:v>B-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>WC</c:v>
+                  <c:v>BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -538,10 +602,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent3">
-                <a:lumMod val="60000"/>
-                <a:lumOff val="40000"/>
-              </a:schemeClr>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -554,7 +615,7 @@
                   <c:v>B-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>WC</c:v>
+                  <c:v>BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -585,11 +646,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2111393080"/>
-        <c:axId val="-2119924456"/>
+        <c:axId val="-2110235304"/>
+        <c:axId val="-2133653160"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2111393080"/>
+        <c:axId val="-2110235304"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -598,7 +659,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2119924456"/>
+        <c:crossAx val="-2133653160"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -606,7 +667,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2119924456"/>
+        <c:axId val="-2133653160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -637,7 +698,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111393080"/>
+        <c:crossAx val="-2110235304"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -719,7 +780,7 @@
                   <c:v>B-R-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BR-WC</c:v>
+                  <c:v>BR-BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -756,7 +817,9 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:schemeClr val="accent2"/>
+              <a:schemeClr val="accent2">
+                <a:lumMod val="50000"/>
+              </a:schemeClr>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -769,7 +832,7 @@
                   <c:v>B-R-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BR-WC</c:v>
+                  <c:v>BR-BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -821,7 +884,7 @@
                   <c:v>B-R-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BR-WC</c:v>
+                  <c:v>BR-BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -858,7 +921,7 @@
           </c:tx>
           <c:spPr>
             <a:solidFill>
-              <a:srgbClr val="C3D69B"/>
+              <a:srgbClr val="008000"/>
             </a:solidFill>
           </c:spPr>
           <c:invertIfNegative val="0"/>
@@ -871,7 +934,7 @@
                   <c:v>B-R-W-C</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>BR-WC</c:v>
+                  <c:v>BR-BWC</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -902,11 +965,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112578920"/>
-        <c:axId val="-2112577512"/>
+        <c:axId val="-2110165944"/>
+        <c:axId val="-2110183752"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112578920"/>
+        <c:axId val="-2110165944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -915,7 +978,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112577512"/>
+        <c:crossAx val="-2110183752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -923,7 +986,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112577512"/>
+        <c:axId val="-2110183752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -953,7 +1016,670 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112578920"/>
+        <c:crossAx val="-2110165944"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Omid 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$12:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>36.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.561</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175.019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210.639</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>241.925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$13:$K$13</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>21.29704582</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.27301571</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>30.31496028</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.58850074</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>45.77452517</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>55.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$14</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lorra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$12:$K$12</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>36.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.561</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175.019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210.639</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>241.925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$14:$K$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.169038514</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.498997017</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>7.369880984</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.5</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>11.04141603</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>22.20637574</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2087459192"/>
+        <c:axId val="-2085034488"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2087459192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KTPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2085034488"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:tickMarkSkip val="1"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2085034488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2087459192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup paperSize="9" orientation="portrait" horizontalDpi="-4" verticalDpi="-4"/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Omid 2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="C0504D"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$21:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>36.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.561</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175.019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210.639</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>241.925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$22:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>39.0852973</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>42.4394</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>51.40291556</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61.37294845</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>106.3239219</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>160.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$A$23</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Lorra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet2!$B$21:$K$21</c:f>
+              <c:numCache>
+                <c:formatCode>0</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>36.99</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>66.632</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>82.845</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>93.561</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>124.817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>173.468</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>175.019</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>206.692</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>210.639</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>241.925</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$B$23:$K$23</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>25.19313333</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>25.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>25.98431502</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>30.85524107</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>47.67003232</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>99.23869173</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2113044488"/>
+        <c:axId val="-2108760584"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2113044488"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KTPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2108760584"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2108760584"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2113044488"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -979,16 +1705,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>749300</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>149352</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>73152</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1010,15 +1736,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>368300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>12700</xdr:rowOff>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>812800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>31496</xdr:rowOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>56896</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1040,14 +1766,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>381000</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>63500</xdr:rowOff>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>25</xdr:row>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>20</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1062,6 +1788,71 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>177800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>127000</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>736600</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>26</xdr:col>
+      <xdr:colOff>355600</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>6350</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1394,8 +2185,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A172" workbookViewId="0">
-      <selection activeCell="K16" sqref="K16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="S24" sqref="S24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1455,7 +2246,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="16">
@@ -1471,7 +2262,7 @@
     </row>
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B10" s="1">
         <v>2.6474121300000002</v>
@@ -1494,7 +2285,7 @@
     <row r="14" spans="1:3" ht="16">
       <c r="A14" s="1"/>
       <c r="B14" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>9</v>
@@ -1524,7 +2315,7 @@
     </row>
     <row r="17" spans="1:3" ht="16">
       <c r="A17" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B17" s="1">
         <v>2.1091406140000002</v>
@@ -1555,4 +2346,709 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M24"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:13" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
+      <c r="M1" s="1"/>
+    </row>
+    <row r="2" spans="1:13" ht="16">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
+        <v>36990</v>
+      </c>
+      <c r="C2" s="1">
+        <v>66632</v>
+      </c>
+      <c r="D2" s="1">
+        <v>82845</v>
+      </c>
+      <c r="E2" s="1">
+        <v>93561</v>
+      </c>
+      <c r="F2" s="1">
+        <v>124817</v>
+      </c>
+      <c r="G2" s="1">
+        <v>173468</v>
+      </c>
+      <c r="H2" s="1">
+        <v>175019</v>
+      </c>
+      <c r="I2" s="1">
+        <v>206692</v>
+      </c>
+      <c r="J2" s="1">
+        <v>210639</v>
+      </c>
+      <c r="K2" s="1">
+        <v>241925</v>
+      </c>
+      <c r="L2" s="1">
+        <v>257986</v>
+      </c>
+      <c r="M2" s="1">
+        <v>277999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1">
+        <v>21.297045820000001</v>
+      </c>
+      <c r="C3" s="1">
+        <v>22.273015709999999</v>
+      </c>
+      <c r="D3" s="1">
+        <v>25</v>
+      </c>
+      <c r="E3" s="1">
+        <v>30.314960280000001</v>
+      </c>
+      <c r="F3" s="1">
+        <v>31</v>
+      </c>
+      <c r="G3" s="1">
+        <v>31</v>
+      </c>
+      <c r="H3" s="1">
+        <v>31.588500740000001</v>
+      </c>
+      <c r="I3" s="1">
+        <v>40</v>
+      </c>
+      <c r="J3" s="1">
+        <v>45.774525169999997</v>
+      </c>
+      <c r="K3" s="1">
+        <v>55</v>
+      </c>
+      <c r="L3" s="1">
+        <v>65</v>
+      </c>
+      <c r="M3" s="1">
+        <v>70.642442590000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="1">
+        <v>6</v>
+      </c>
+      <c r="C4" s="1">
+        <v>6</v>
+      </c>
+      <c r="D4" s="1">
+        <v>6.1690385140000004</v>
+      </c>
+      <c r="E4" s="1">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1">
+        <v>6.4989970169999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>7.3698809839999999</v>
+      </c>
+      <c r="H4" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="I4" s="1">
+        <v>11.041416030000001</v>
+      </c>
+      <c r="J4" s="1">
+        <v>12</v>
+      </c>
+      <c r="K4" s="1">
+        <v>22.206375739999999</v>
+      </c>
+      <c r="L4" s="1">
+        <v>44.834804910000003</v>
+      </c>
+      <c r="M4" s="1"/>
+    </row>
+    <row r="5" spans="1:13" ht="16">
+      <c r="A5" s="1"/>
+      <c r="B5" s="1"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+    </row>
+    <row r="6" spans="1:13" ht="16">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
+      <c r="G6" s="1"/>
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+    </row>
+    <row r="7" spans="1:13" ht="16">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1">
+        <v>36990</v>
+      </c>
+      <c r="C7" s="1">
+        <v>66632</v>
+      </c>
+      <c r="D7" s="1">
+        <v>82845</v>
+      </c>
+      <c r="E7" s="1">
+        <v>93561</v>
+      </c>
+      <c r="F7" s="1">
+        <v>124817</v>
+      </c>
+      <c r="G7" s="1">
+        <v>173468</v>
+      </c>
+      <c r="H7" s="1">
+        <v>175019</v>
+      </c>
+      <c r="I7" s="1">
+        <v>206692</v>
+      </c>
+      <c r="J7" s="1">
+        <v>210639</v>
+      </c>
+      <c r="K7" s="1">
+        <v>241925</v>
+      </c>
+      <c r="L7" s="1">
+        <v>257986</v>
+      </c>
+      <c r="M7" s="1">
+        <v>277999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="16">
+      <c r="A8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="1">
+        <v>39.085297300000001</v>
+      </c>
+      <c r="C8" s="1">
+        <v>42.439399999999999</v>
+      </c>
+      <c r="D8" s="1">
+        <v>47</v>
+      </c>
+      <c r="E8" s="1">
+        <v>51.402915559999997</v>
+      </c>
+      <c r="F8" s="1">
+        <v>51</v>
+      </c>
+      <c r="G8" s="1">
+        <v>60</v>
+      </c>
+      <c r="H8" s="1">
+        <v>61.372948450000003</v>
+      </c>
+      <c r="I8" s="1">
+        <v>100</v>
+      </c>
+      <c r="J8" s="1">
+        <v>106.3239219</v>
+      </c>
+      <c r="K8" s="1">
+        <v>160</v>
+      </c>
+      <c r="L8" s="1">
+        <v>170</v>
+      </c>
+      <c r="M8" s="1">
+        <v>187.4820105</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="1">
+        <v>25</v>
+      </c>
+      <c r="C9" s="1">
+        <v>25</v>
+      </c>
+      <c r="D9" s="1">
+        <v>25.193133329999998</v>
+      </c>
+      <c r="E9" s="1">
+        <v>25</v>
+      </c>
+      <c r="F9" s="1">
+        <v>25.98431502</v>
+      </c>
+      <c r="G9" s="1">
+        <v>30.855241070000002</v>
+      </c>
+      <c r="H9" s="1">
+        <v>31</v>
+      </c>
+      <c r="I9" s="1">
+        <v>47.670032319999997</v>
+      </c>
+      <c r="J9" s="1">
+        <v>50</v>
+      </c>
+      <c r="K9" s="1">
+        <v>99.238691729999999</v>
+      </c>
+      <c r="L9" s="1">
+        <v>201.636619</v>
+      </c>
+      <c r="M9" s="1"/>
+    </row>
+    <row r="11" spans="1:13" ht="16">
+      <c r="A11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
+      <c r="H11" s="3"/>
+      <c r="I11" s="3"/>
+      <c r="J11" s="3"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+      <c r="M11" s="3"/>
+    </row>
+    <row r="12" spans="1:13">
+      <c r="A12" s="3"/>
+      <c r="B12" s="6">
+        <f>B2/1000</f>
+        <v>36.99</v>
+      </c>
+      <c r="C12" s="6">
+        <f t="shared" ref="C12:M12" si="0">C2/1000</f>
+        <v>66.632000000000005</v>
+      </c>
+      <c r="D12" s="6">
+        <f t="shared" si="0"/>
+        <v>82.844999999999999</v>
+      </c>
+      <c r="E12" s="6">
+        <f t="shared" si="0"/>
+        <v>93.561000000000007</v>
+      </c>
+      <c r="F12" s="6">
+        <f t="shared" si="0"/>
+        <v>124.81699999999999</v>
+      </c>
+      <c r="G12" s="6">
+        <f t="shared" si="0"/>
+        <v>173.46799999999999</v>
+      </c>
+      <c r="H12" s="6">
+        <f t="shared" si="0"/>
+        <v>175.01900000000001</v>
+      </c>
+      <c r="I12" s="6">
+        <f t="shared" si="0"/>
+        <v>206.69200000000001</v>
+      </c>
+      <c r="J12" s="6">
+        <f t="shared" si="0"/>
+        <v>210.63900000000001</v>
+      </c>
+      <c r="K12" s="6">
+        <f t="shared" si="0"/>
+        <v>241.92500000000001</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="0"/>
+        <v>257.98599999999999</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="0"/>
+        <v>277.99900000000002</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="16">
+      <c r="A13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B13" s="2">
+        <v>21.297045820000001</v>
+      </c>
+      <c r="C13" s="2">
+        <v>22.273015709999999</v>
+      </c>
+      <c r="D13" s="2">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2">
+        <v>30.314960280000001</v>
+      </c>
+      <c r="F13" s="2">
+        <v>31</v>
+      </c>
+      <c r="G13" s="2">
+        <v>31</v>
+      </c>
+      <c r="H13" s="2">
+        <v>31.588500740000001</v>
+      </c>
+      <c r="I13" s="2">
+        <v>40</v>
+      </c>
+      <c r="J13" s="2">
+        <v>45.774525169999997</v>
+      </c>
+      <c r="K13" s="2">
+        <v>55</v>
+      </c>
+      <c r="L13" s="2">
+        <v>65</v>
+      </c>
+      <c r="M13" s="2">
+        <v>70.642442590000002</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="16">
+      <c r="A14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B14" s="2">
+        <v>6</v>
+      </c>
+      <c r="C14" s="2">
+        <v>6</v>
+      </c>
+      <c r="D14" s="2">
+        <v>6.1690385140000004</v>
+      </c>
+      <c r="E14" s="2">
+        <v>6</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6.4989970169999998</v>
+      </c>
+      <c r="G14" s="2">
+        <v>7.3698809839999999</v>
+      </c>
+      <c r="H14" s="2">
+        <v>7.5</v>
+      </c>
+      <c r="I14" s="2">
+        <v>11.041416030000001</v>
+      </c>
+      <c r="J14" s="2">
+        <v>12</v>
+      </c>
+      <c r="K14" s="2">
+        <v>22.206375739999999</v>
+      </c>
+      <c r="L14" s="2">
+        <v>44.834804910000003</v>
+      </c>
+      <c r="M14" s="2"/>
+    </row>
+    <row r="15" spans="1:13">
+      <c r="B15">
+        <f>B13/B14</f>
+        <v>3.5495076366666667</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:M15" si="1">C13/C14</f>
+        <v>3.7121692849999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>4.0524953675139264</v>
+      </c>
+      <c r="E15">
+        <f t="shared" si="1"/>
+        <v>5.0524933800000005</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>4.7699667993246599</v>
+      </c>
+      <c r="G15">
+        <f t="shared" si="1"/>
+        <v>4.2063094461499384</v>
+      </c>
+      <c r="H15">
+        <f t="shared" si="1"/>
+        <v>4.211800098666667</v>
+      </c>
+      <c r="I15">
+        <f t="shared" si="1"/>
+        <v>3.6227237422553671</v>
+      </c>
+      <c r="J15">
+        <f t="shared" si="1"/>
+        <v>3.8145437641666664</v>
+      </c>
+      <c r="K15">
+        <f t="shared" si="1"/>
+        <v>2.47676616139253</v>
+      </c>
+      <c r="L15">
+        <f t="shared" si="1"/>
+        <v>1.4497665403134681</v>
+      </c>
+      <c r="M15" t="e">
+        <f t="shared" si="1"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="16">
+      <c r="A20" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B20" s="5"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
+      <c r="K20" s="5"/>
+      <c r="L20" s="5"/>
+      <c r="M20" s="5"/>
+    </row>
+    <row r="21" spans="1:13">
+      <c r="A21" s="5"/>
+      <c r="B21" s="7">
+        <f>B7/1000</f>
+        <v>36.99</v>
+      </c>
+      <c r="C21" s="7">
+        <f t="shared" ref="C21:M21" si="2">C7/1000</f>
+        <v>66.632000000000005</v>
+      </c>
+      <c r="D21" s="7">
+        <f t="shared" si="2"/>
+        <v>82.844999999999999</v>
+      </c>
+      <c r="E21" s="7">
+        <f t="shared" si="2"/>
+        <v>93.561000000000007</v>
+      </c>
+      <c r="F21" s="7">
+        <f t="shared" si="2"/>
+        <v>124.81699999999999</v>
+      </c>
+      <c r="G21" s="7">
+        <f t="shared" si="2"/>
+        <v>173.46799999999999</v>
+      </c>
+      <c r="H21" s="7">
+        <f t="shared" si="2"/>
+        <v>175.01900000000001</v>
+      </c>
+      <c r="I21" s="7">
+        <f t="shared" si="2"/>
+        <v>206.69200000000001</v>
+      </c>
+      <c r="J21" s="7">
+        <f t="shared" si="2"/>
+        <v>210.63900000000001</v>
+      </c>
+      <c r="K21" s="7">
+        <f t="shared" si="2"/>
+        <v>241.92500000000001</v>
+      </c>
+      <c r="L21" s="7">
+        <f t="shared" si="2"/>
+        <v>257.98599999999999</v>
+      </c>
+      <c r="M21" s="7">
+        <f t="shared" si="2"/>
+        <v>277.99900000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="16">
+      <c r="A22" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B22" s="4">
+        <v>39.085297300000001</v>
+      </c>
+      <c r="C22" s="4">
+        <v>42.439399999999999</v>
+      </c>
+      <c r="D22" s="4">
+        <v>47</v>
+      </c>
+      <c r="E22" s="4">
+        <v>51.402915559999997</v>
+      </c>
+      <c r="F22" s="4">
+        <v>51</v>
+      </c>
+      <c r="G22" s="4">
+        <v>60</v>
+      </c>
+      <c r="H22" s="4">
+        <v>61.372948450000003</v>
+      </c>
+      <c r="I22" s="4">
+        <v>100</v>
+      </c>
+      <c r="J22" s="4">
+        <v>106.3239219</v>
+      </c>
+      <c r="K22" s="4">
+        <v>160</v>
+      </c>
+      <c r="L22" s="4">
+        <v>170</v>
+      </c>
+      <c r="M22" s="4">
+        <v>187.4820105</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="16">
+      <c r="A23" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B23" s="4">
+        <v>25</v>
+      </c>
+      <c r="C23" s="4">
+        <v>25</v>
+      </c>
+      <c r="D23" s="4">
+        <v>25.193133329999998</v>
+      </c>
+      <c r="E23" s="4">
+        <v>25</v>
+      </c>
+      <c r="F23" s="4">
+        <v>25.98431502</v>
+      </c>
+      <c r="G23" s="4">
+        <v>30.855241070000002</v>
+      </c>
+      <c r="H23" s="4">
+        <v>31</v>
+      </c>
+      <c r="I23" s="4">
+        <v>47.670032319999997</v>
+      </c>
+      <c r="J23" s="4">
+        <v>50</v>
+      </c>
+      <c r="K23" s="4">
+        <v>99.238691729999999</v>
+      </c>
+      <c r="L23" s="4">
+        <v>201.636619</v>
+      </c>
+      <c r="M23" s="4"/>
+    </row>
+    <row r="24" spans="1:13">
+      <c r="B24">
+        <f>B22/B23</f>
+        <v>1.563411892</v>
+      </c>
+      <c r="C24">
+        <f t="shared" ref="C24:M24" si="3">C22/C23</f>
+        <v>1.697576</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="3"/>
+        <v>1.8655877133009244</v>
+      </c>
+      <c r="E24">
+        <f t="shared" si="3"/>
+        <v>2.0561166223999998</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>1.9627225101275732</v>
+      </c>
+      <c r="G24">
+        <f t="shared" si="3"/>
+        <v>1.944564291812872</v>
+      </c>
+      <c r="H24">
+        <f t="shared" si="3"/>
+        <v>1.9797725306451615</v>
+      </c>
+      <c r="I24">
+        <f t="shared" si="3"/>
+        <v>2.0977539794544029</v>
+      </c>
+      <c r="J24">
+        <f t="shared" si="3"/>
+        <v>2.1264784379999999</v>
+      </c>
+      <c r="K24">
+        <f t="shared" si="3"/>
+        <v>1.6122743781761462</v>
+      </c>
+      <c r="L24">
+        <f t="shared" si="3"/>
+        <v>0.84310082584751134</v>
+      </c>
+      <c r="M24" t="e">
+        <f t="shared" si="3"/>
+        <v>#DIV/0!</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
New results in xlsx file
</commit_message>
<xml_diff>
--- a/figs/results.xlsx
+++ b/figs/results.xlsx
@@ -1,14 +1,17 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27629"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-36680" yWindow="680" windowWidth="38400" windowHeight="16920" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3200" yWindow="1480" windowWidth="35200" windowHeight="22060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="TXLatency" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -20,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
   <si>
     <t>Read</t>
   </si>
@@ -63,12 +66,66 @@
   <si>
     <t>Lorra</t>
   </si>
+  <si>
+    <t>single transaction</t>
+  </si>
+  <si>
+    <t>omid LL write</t>
+  </si>
+  <si>
+    <t>beign</t>
+  </si>
+  <si>
+    <t>hbase</t>
+  </si>
+  <si>
+    <t>commit</t>
+  </si>
+  <si>
+    <t>single read</t>
+  </si>
+  <si>
+    <t>lorra (singletons)</t>
+  </si>
+  <si>
+    <t>omid LL</t>
+  </si>
+  <si>
+    <t>begin</t>
+  </si>
+  <si>
+    <t>TX 10</t>
+  </si>
+  <si>
+    <t>lorra (checkAndMutate)</t>
+  </si>
+  <si>
+    <t>omid LL (Put)</t>
+  </si>
+  <si>
+    <t>omid</t>
+  </si>
+  <si>
+    <t>omidLL</t>
+  </si>
+  <si>
+    <t>omidLocal</t>
+  </si>
+  <si>
+    <t>lorra</t>
+  </si>
+  <si>
+    <t>single write</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0"/>
+  </numFmts>
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -103,6 +160,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13.2"/>
+      <color rgb="FF000000"/>
+      <name val="Inconsolata"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -133,8 +195,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="17">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="23">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -151,18 +213,25 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+  <cellXfs count="9">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="17">
+  <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -171,6 +240,9 @@
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -179,7 +251,10 @@
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
@@ -258,7 +333,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$3:$C$3</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.3428831454</c:v>
@@ -311,7 +386,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$4:$C$4</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.458520434</c:v>
@@ -364,7 +439,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$5:$C$5</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.005278454431</c:v>
@@ -386,11 +461,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2132884136"/>
-        <c:axId val="-2133590664"/>
+        <c:axId val="-2110059448"/>
+        <c:axId val="-2110054904"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2132884136"/>
+        <c:axId val="-2110059448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -399,7 +474,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133590664"/>
+        <c:crossAx val="-2110054904"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -407,7 +482,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133590664"/>
+        <c:axId val="-2110054904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -434,11 +509,1192 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2132884136"/>
+        <c:crossAx val="-2110059448"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart10.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TX Size 1</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>288.537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>301.258</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>360.337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$3:$U$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>18.75496056</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20.35794558</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>22.12859037</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>32.65668377</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>45.78419551</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>60.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>73.09440964</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$2:$U$2</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>115.373</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>288.537</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>301.258</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>360.337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$4:$U$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>5.8</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.9</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>5.908033275</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.9</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4.9</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.987738946999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8.95559215</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2077107480"/>
+        <c:axId val="-2077106072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2077107480"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KTPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077106072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2077106072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="120.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077107480"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart11.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TX Size</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 5</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$10:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.258</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360.337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$11:$T$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>32.008</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>33.26613333</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.40316867</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>47.17763485</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>63.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>67.3873265</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100.8789393</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$10:$T$10</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.258</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>360.337</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$12:$T$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>18.41479408</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>18.41479408</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>18.41479408</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>18.41479408</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>18.41479408</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>23.02344454</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2077673976"/>
+        <c:axId val="-2077278392"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2077673976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KTPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077278392"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2077278392"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2077673976"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart12.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TX</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Size 10</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$19</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$18:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.258</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$19:$S$19</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>41.087</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>44.39037838</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>46.75394286</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>57.09780995000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>70.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>76.16235616</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>109.7466319</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>TXLatency!$L$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="4F81BD"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>TXLatency!$M$18:$S$18</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>35.886</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>63.909</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>108.821</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>165.487</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>256.925</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>269.891</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>301.258</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>TXLatency!$M$20:$S$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>37.55323243</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>37.55323243</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>37.55323243</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>37.55323243</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>37.55323243</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>39.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2061912760"/>
+        <c:axId val="-2061909976"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2061912760"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>KTPS</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2061909976"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2061909976"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2061912760"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>lorra</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>single read</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>single write</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TX 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TX 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$B$2:$B$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>7.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet5!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet5!$A$2:$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>single read</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>single write</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>TX 5</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>TX 10</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet5!$C$2:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:axId val="-2072820568"/>
+        <c:axId val="-2075784856"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2072820568"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2075784856"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2075784856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2072820568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -522,7 +1778,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$9:$C$9</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.4472012821</c:v>
@@ -574,7 +1830,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$10:$C$10</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.64741213</c:v>
@@ -624,7 +1880,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$11:$C$11</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.446877811</c:v>
@@ -646,11 +1902,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2110235304"/>
-        <c:axId val="-2133653160"/>
+        <c:axId val="-2109993800"/>
+        <c:axId val="-2109946392"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110235304"/>
+        <c:axId val="-2109993800"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -659,7 +1915,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2133653160"/>
+        <c:crossAx val="-2109946392"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -667,7 +1923,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2133653160"/>
+        <c:axId val="-2109946392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -694,11 +1950,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110235304"/>
+        <c:crossAx val="-2109993800"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -789,7 +2045,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$15:$C$15</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>0.4520979381</c:v>
@@ -841,7 +2097,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$16:$C$16</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>1.758736035</c:v>
@@ -893,7 +2149,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$17:$C$17</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.109140614</c:v>
@@ -943,7 +2199,7 @@
             <c:numRef>
               <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
                   <c:v>2.418978542</c:v>
@@ -965,11 +2221,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2110165944"/>
-        <c:axId val="-2110183752"/>
+        <c:axId val="-2109936408"/>
+        <c:axId val="-2109926600"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110165944"/>
+        <c:axId val="-2109936408"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -978,7 +2234,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110183752"/>
+        <c:crossAx val="-2109926600"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -986,7 +2242,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110183752"/>
+        <c:axId val="-2109926600"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1012,11 +2268,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110165944"/>
+        <c:crossAx val="-2109936408"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1125,7 +2381,7 @@
             <c:numRef>
               <c:f>Sheet2!$B$13:$K$13</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>21.29704582</c:v>
@@ -1229,7 +2485,7 @@
             <c:numRef>
               <c:f>Sheet2!$B$14:$K$14</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>6.0</c:v>
@@ -1276,11 +2532,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2087459192"/>
-        <c:axId val="-2085034488"/>
+        <c:axId val="-2131827368"/>
+        <c:axId val="-2131790584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2087459192"/>
+        <c:axId val="-2131827368"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1309,7 +2565,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2085034488"/>
+        <c:crossAx val="-2131790584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1318,7 +2574,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2085034488"/>
+        <c:axId val="-2131790584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1344,11 +2600,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2087459192"/>
+        <c:crossAx val="-2131827368"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1457,7 +2713,7 @@
             <c:numRef>
               <c:f>Sheet2!$B$22:$K$22</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>39.0852973</c:v>
@@ -1561,7 +2817,7 @@
             <c:numRef>
               <c:f>Sheet2!$B$23:$K$23</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
+                <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>25.0</c:v>
@@ -1608,11 +2864,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2113044488"/>
-        <c:axId val="-2108760584"/>
+        <c:axId val="-2111991624"/>
+        <c:axId val="-2111929880"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2113044488"/>
+        <c:axId val="-2111991624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1641,7 +2897,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2108760584"/>
+        <c:crossAx val="-2111929880"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1649,7 +2905,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2108760584"/>
+        <c:axId val="-2111929880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1675,11 +2931,11 @@
           <c:layout/>
           <c:overlay val="0"/>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2113044488"/>
+        <c:crossAx val="-2111991624"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1693,6 +2949,1065 @@
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Single Write</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$3</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$3:$C$3</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.26</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$4</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hbase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$4:$C$4</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>3.63</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.04</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$5</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>commit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$2:$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL write</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$5:$C$5</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>6.81</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2112840744"/>
+        <c:axId val="-2112502312"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2112840744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2112502312"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2112502312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2112840744"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Single Read</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$11</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>beign</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$9:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$11:$C$11</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.27</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$12</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hbase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$9:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$12:$C$12</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.51</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.66</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$13</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>commit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$9:$C$10</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (singletons)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$13:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2080155560"/>
+        <c:axId val="-2111993896"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2080155560"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2111993896"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2111993896"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="10.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080155560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart8.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TX Size</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> 5</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$20</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>begin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$18:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$20:$C$20</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$21</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hbase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$18:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$21:$C$21</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>13.57</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.79</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>commit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$18:$C$19</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$22:$C$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>12.85</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>12.06</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2080025416"/>
+        <c:axId val="-2128165112"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2080025416"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2128165112"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2128165112"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="60.0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2080025416"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart9.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TX Size 10</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="stacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$27</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>begin</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$27:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>0.33</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.29</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$28</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>hbase</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$28:$C$28</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>27.14</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>17.57</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet3!$A$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>commit</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>Sheet3!$B$25:$C$26</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>lorra (checkAndMutate)</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>omid LL (Put)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet3!$B$29:$C$29</c:f>
+              <c:numCache>
+                <c:formatCode>0.0</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>23.68</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>22.86</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="-2112594856"/>
+        <c:axId val="-2126249720"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2112594856"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2126249720"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2126249720"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" vert="horz"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>[msec]</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2112594856"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr sz="2000"/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
   <c:printSettings>
     <c:headerFooter/>
     <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
@@ -1853,6 +4168,261 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>800100</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>196850</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>749300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>82550</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>317500</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>762000</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>95250</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>215900</xdr:colOff>
+      <xdr:row>34</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>673100</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>292100</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>596900</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>444500</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>12700</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>63500</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>622300</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>101600</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2352,7 +4922,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
@@ -3051,4 +5621,1059 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C29"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="23.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+    </row>
+    <row r="2" spans="1:3" ht="16">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="1">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="1">
+        <v>3.63</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.04</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="1">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6.81</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="16">
+      <c r="A6" s="1"/>
+      <c r="B6" s="1"/>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" spans="1:3" ht="16">
+      <c r="A7" s="1"/>
+      <c r="B7" s="1"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" spans="1:3" ht="16">
+      <c r="A8" s="1"/>
+      <c r="B8" s="1"/>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" spans="1:3" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+    </row>
+    <row r="10" spans="1:3" ht="16">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="1">
+        <v>0</v>
+      </c>
+      <c r="C11" s="1">
+        <v>0.27</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" ht="16">
+      <c r="A12" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="1">
+        <v>1.51</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1.66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="16">
+      <c r="A13" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" s="1">
+        <v>0</v>
+      </c>
+      <c r="C13" s="1">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="16">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+    </row>
+    <row r="15" spans="1:3" ht="16">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+    </row>
+    <row r="16" spans="1:3" ht="16">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+    </row>
+    <row r="17" spans="1:3" ht="16">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+    </row>
+    <row r="18" spans="1:3" ht="16">
+      <c r="A18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+    </row>
+    <row r="19" spans="1:3" ht="16">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B20" s="1">
+        <v>0.33</v>
+      </c>
+      <c r="C20" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B21" s="1">
+        <v>13.57</v>
+      </c>
+      <c r="C21" s="1">
+        <v>8.7899999999999991</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="16">
+      <c r="A22" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" s="1">
+        <v>12.85</v>
+      </c>
+      <c r="C22" s="1">
+        <v>12.06</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="16">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+    </row>
+    <row r="24" spans="1:3" ht="16">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+    </row>
+    <row r="25" spans="1:3" ht="16">
+      <c r="A25" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+    </row>
+    <row r="26" spans="1:3" ht="16">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="17">
+      <c r="A27" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B27" s="8">
+        <v>0.33</v>
+      </c>
+      <c r="C27" s="8">
+        <v>0.28999999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="17">
+      <c r="A28" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B28" s="8">
+        <v>27.14</v>
+      </c>
+      <c r="C28" s="8">
+        <v>17.57</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="16">
+      <c r="A29" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B29" s="1">
+        <v>23.68</v>
+      </c>
+      <c r="C29" s="1">
+        <v>22.86</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U26"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="O41" sqref="O41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:21" ht="16">
+      <c r="A1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+    </row>
+    <row r="2" spans="1:21" ht="16">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1">
+        <v>35886</v>
+      </c>
+      <c r="C2" s="1">
+        <v>52809</v>
+      </c>
+      <c r="D2" s="1">
+        <v>63909</v>
+      </c>
+      <c r="E2" s="1">
+        <v>108821</v>
+      </c>
+      <c r="F2" s="1">
+        <v>115373</v>
+      </c>
+      <c r="G2" s="1">
+        <v>165487</v>
+      </c>
+      <c r="H2" s="1">
+        <v>269891</v>
+      </c>
+      <c r="I2" s="1">
+        <v>288537</v>
+      </c>
+      <c r="J2" s="1">
+        <v>301258</v>
+      </c>
+      <c r="K2" s="1">
+        <v>360337</v>
+      </c>
+      <c r="M2">
+        <f>B2/1000</f>
+        <v>35.886000000000003</v>
+      </c>
+      <c r="N2">
+        <f>D2/1000</f>
+        <v>63.908999999999999</v>
+      </c>
+      <c r="O2">
+        <f>E2/1000</f>
+        <v>108.821</v>
+      </c>
+      <c r="P2">
+        <f>F2/1000</f>
+        <v>115.373</v>
+      </c>
+      <c r="Q2">
+        <f>G2/1000</f>
+        <v>165.48699999999999</v>
+      </c>
+      <c r="R2">
+        <f>H2/1000</f>
+        <v>269.89100000000002</v>
+      </c>
+      <c r="S2">
+        <f>I2/1000</f>
+        <v>288.53699999999998</v>
+      </c>
+      <c r="T2">
+        <f>J2/1000</f>
+        <v>301.25799999999998</v>
+      </c>
+      <c r="U2">
+        <f>K2/1000</f>
+        <v>360.33699999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" ht="16">
+      <c r="A3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" s="1">
+        <v>18754.96056</v>
+      </c>
+      <c r="C3" s="1">
+        <v>20000</v>
+      </c>
+      <c r="D3" s="1">
+        <v>20357.94558</v>
+      </c>
+      <c r="E3" s="1">
+        <v>22128.590370000002</v>
+      </c>
+      <c r="F3" s="1">
+        <v>23000</v>
+      </c>
+      <c r="G3" s="1">
+        <v>32656.68377</v>
+      </c>
+      <c r="H3" s="1">
+        <v>45784.195509999998</v>
+      </c>
+      <c r="I3" s="1">
+        <v>60000</v>
+      </c>
+      <c r="J3" s="1">
+        <v>73094.409639999998</v>
+      </c>
+      <c r="K3" s="1"/>
+      <c r="L3" t="s">
+        <v>26</v>
+      </c>
+      <c r="M3">
+        <f>B3/1000</f>
+        <v>18.754960560000001</v>
+      </c>
+      <c r="N3">
+        <f>D3/1000</f>
+        <v>20.357945579999999</v>
+      </c>
+      <c r="O3">
+        <f>E3/1000</f>
+        <v>22.128590370000001</v>
+      </c>
+      <c r="P3">
+        <f>F3/1000</f>
+        <v>23</v>
+      </c>
+      <c r="Q3">
+        <f>G3/1000</f>
+        <v>32.656683770000001</v>
+      </c>
+      <c r="R3">
+        <f>H3/1000</f>
+        <v>45.784195509999996</v>
+      </c>
+      <c r="S3">
+        <f>I3/1000</f>
+        <v>60</v>
+      </c>
+      <c r="T3">
+        <f>J3/1000</f>
+        <v>73.094409639999995</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" ht="16">
+      <c r="A4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4" s="1">
+        <v>5800</v>
+      </c>
+      <c r="C4" s="1">
+        <v>5834.124339</v>
+      </c>
+      <c r="D4" s="1">
+        <v>5900</v>
+      </c>
+      <c r="E4" s="1">
+        <v>5900</v>
+      </c>
+      <c r="F4" s="1">
+        <v>5908.0332749999998</v>
+      </c>
+      <c r="G4" s="1">
+        <v>4900</v>
+      </c>
+      <c r="H4" s="1">
+        <v>4900</v>
+      </c>
+      <c r="I4" s="1">
+        <v>4987.7389469999998</v>
+      </c>
+      <c r="J4" s="1">
+        <v>6000</v>
+      </c>
+      <c r="K4" s="1">
+        <v>8955.5921500000004</v>
+      </c>
+      <c r="L4" t="s">
+        <v>21</v>
+      </c>
+      <c r="M4">
+        <f>B4/1000</f>
+        <v>5.8</v>
+      </c>
+      <c r="N4">
+        <f>D4/1000</f>
+        <v>5.9</v>
+      </c>
+      <c r="O4">
+        <f>E4/1000</f>
+        <v>5.9</v>
+      </c>
+      <c r="P4">
+        <f>F4/1000</f>
+        <v>5.9080332750000002</v>
+      </c>
+      <c r="Q4">
+        <f>G4/1000</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="R4">
+        <f>H4/1000</f>
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="S4">
+        <f>I4/1000</f>
+        <v>4.9877389469999995</v>
+      </c>
+      <c r="T4">
+        <f>J4/1000</f>
+        <v>6</v>
+      </c>
+      <c r="U4">
+        <f>K4/1000</f>
+        <v>8.9555921500000011</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="16">
+      <c r="A5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="1">
+        <v>6800</v>
+      </c>
+      <c r="C5" s="1">
+        <v>6842.2129759999998</v>
+      </c>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1">
+        <v>6489.8604500000001</v>
+      </c>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1">
+        <v>5547.134892</v>
+      </c>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1">
+        <v>8864.7199330000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="16">
+      <c r="A9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+      <c r="I9" s="1"/>
+    </row>
+    <row r="10" spans="1:21" ht="16">
+      <c r="A10" s="1"/>
+      <c r="B10" s="1">
+        <v>35886</v>
+      </c>
+      <c r="C10" s="1">
+        <v>63909</v>
+      </c>
+      <c r="D10" s="1">
+        <v>108821</v>
+      </c>
+      <c r="E10" s="1">
+        <v>165487</v>
+      </c>
+      <c r="F10" s="1">
+        <v>256925</v>
+      </c>
+      <c r="G10" s="1">
+        <v>269891</v>
+      </c>
+      <c r="H10" s="1">
+        <v>301258</v>
+      </c>
+      <c r="I10" s="1">
+        <v>360337</v>
+      </c>
+      <c r="M10">
+        <f>B10/1000</f>
+        <v>35.886000000000003</v>
+      </c>
+      <c r="N10">
+        <f t="shared" ref="N10:T10" si="0">C10/1000</f>
+        <v>63.908999999999999</v>
+      </c>
+      <c r="O10">
+        <f t="shared" si="0"/>
+        <v>108.821</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="0"/>
+        <v>165.48699999999999</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="0"/>
+        <v>256.92500000000001</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="0"/>
+        <v>269.89100000000002</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="0"/>
+        <v>301.25799999999998</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="0"/>
+        <v>360.33699999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:21" ht="16">
+      <c r="A11" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B11" s="1">
+        <v>32008</v>
+      </c>
+      <c r="C11" s="1">
+        <v>33266.133329999997</v>
+      </c>
+      <c r="D11" s="1">
+        <v>37403.168669999999</v>
+      </c>
+      <c r="E11" s="1">
+        <v>47177.634850000002</v>
+      </c>
+      <c r="F11" s="1">
+        <v>63000</v>
+      </c>
+      <c r="G11" s="1">
+        <v>67387.326499999996</v>
+      </c>
+      <c r="H11" s="1">
+        <v>100878.9393</v>
+      </c>
+      <c r="I11" s="1"/>
+      <c r="L11" t="s">
+        <v>26</v>
+      </c>
+      <c r="M11">
+        <f t="shared" ref="M11:M12" si="1">B11/1000</f>
+        <v>32.008000000000003</v>
+      </c>
+      <c r="N11">
+        <f t="shared" ref="N11:N12" si="2">C11/1000</f>
+        <v>33.266133329999995</v>
+      </c>
+      <c r="O11">
+        <f t="shared" ref="O11:O12" si="3">D11/1000</f>
+        <v>37.403168669999999</v>
+      </c>
+      <c r="P11">
+        <f t="shared" ref="P11:P12" si="4">E11/1000</f>
+        <v>47.177634850000004</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" ref="Q11:Q12" si="5">F11/1000</f>
+        <v>63</v>
+      </c>
+      <c r="R11">
+        <f t="shared" ref="R11:R12" si="6">G11/1000</f>
+        <v>67.3873265</v>
+      </c>
+      <c r="S11">
+        <f t="shared" ref="S11:T12" si="7">H11/1000</f>
+        <v>100.8789393</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="16">
+      <c r="A12" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B12" s="1">
+        <v>18414.79408</v>
+      </c>
+      <c r="C12" s="1">
+        <v>18414.79408</v>
+      </c>
+      <c r="D12" s="1">
+        <v>18414.79408</v>
+      </c>
+      <c r="E12" s="1">
+        <v>18414.79408</v>
+      </c>
+      <c r="F12" s="1">
+        <v>18414.79408</v>
+      </c>
+      <c r="G12" s="1">
+        <v>20000</v>
+      </c>
+      <c r="H12" s="1">
+        <v>23000</v>
+      </c>
+      <c r="I12" s="1">
+        <v>23023.44454</v>
+      </c>
+      <c r="L12" t="s">
+        <v>21</v>
+      </c>
+      <c r="M12">
+        <f t="shared" si="1"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="N12">
+        <f t="shared" si="2"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="O12">
+        <f t="shared" si="3"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="P12">
+        <f t="shared" si="4"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="5"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="R12">
+        <f t="shared" si="6"/>
+        <v>20</v>
+      </c>
+      <c r="S12">
+        <f t="shared" si="7"/>
+        <v>23</v>
+      </c>
+      <c r="T12">
+        <f t="shared" si="7"/>
+        <v>23.02344454</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="16">
+      <c r="A13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" s="1">
+        <v>19528.699280000001</v>
+      </c>
+      <c r="C13" s="1">
+        <v>19528.699280000001</v>
+      </c>
+      <c r="D13" s="1">
+        <v>19528.699280000001</v>
+      </c>
+      <c r="E13" s="1">
+        <v>19528.699280000001</v>
+      </c>
+      <c r="F13" s="1">
+        <v>19528.699280000001</v>
+      </c>
+      <c r="G13" s="1">
+        <v>21000</v>
+      </c>
+      <c r="H13" s="1">
+        <v>25000</v>
+      </c>
+      <c r="I13" s="1">
+        <v>25099.169600000001</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" ht="16">
+      <c r="A18" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="1"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="M18">
+        <f>B19/1000</f>
+        <v>35.886000000000003</v>
+      </c>
+      <c r="N18">
+        <f>C19/1000</f>
+        <v>63.908999999999999</v>
+      </c>
+      <c r="O18">
+        <f>D19/1000</f>
+        <v>108.821</v>
+      </c>
+      <c r="P18">
+        <f>E19/1000</f>
+        <v>165.48699999999999</v>
+      </c>
+      <c r="Q18">
+        <f>F19/1000</f>
+        <v>256.92500000000001</v>
+      </c>
+      <c r="R18">
+        <f>G19/1000</f>
+        <v>269.89100000000002</v>
+      </c>
+      <c r="S18">
+        <f>H19/1000</f>
+        <v>301.25799999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="16">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1">
+        <v>35886</v>
+      </c>
+      <c r="C19" s="1">
+        <v>63909</v>
+      </c>
+      <c r="D19" s="1">
+        <v>108821</v>
+      </c>
+      <c r="E19" s="1">
+        <v>165487</v>
+      </c>
+      <c r="F19" s="1">
+        <v>256925</v>
+      </c>
+      <c r="G19" s="1">
+        <v>269891</v>
+      </c>
+      <c r="H19" s="1">
+        <v>301258</v>
+      </c>
+      <c r="I19" s="1">
+        <v>360337</v>
+      </c>
+      <c r="L19" t="s">
+        <v>26</v>
+      </c>
+      <c r="M19">
+        <f>B20/1000</f>
+        <v>41.087000000000003</v>
+      </c>
+      <c r="N19">
+        <f t="shared" ref="N19:S20" si="8">C20/1000</f>
+        <v>44.390378380000001</v>
+      </c>
+      <c r="O19">
+        <f t="shared" si="8"/>
+        <v>46.753942860000002</v>
+      </c>
+      <c r="P19">
+        <f t="shared" si="8"/>
+        <v>57.097809950000006</v>
+      </c>
+      <c r="Q19">
+        <f t="shared" si="8"/>
+        <v>70</v>
+      </c>
+      <c r="R19">
+        <f t="shared" si="8"/>
+        <v>76.162356160000002</v>
+      </c>
+      <c r="S19">
+        <f t="shared" si="8"/>
+        <v>109.7466319</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="16">
+      <c r="A20" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B20" s="1">
+        <v>41087</v>
+      </c>
+      <c r="C20" s="1">
+        <v>44390.378380000002</v>
+      </c>
+      <c r="D20" s="1">
+        <v>46753.942860000003</v>
+      </c>
+      <c r="E20" s="1">
+        <v>57097.809950000003</v>
+      </c>
+      <c r="F20" s="1">
+        <v>70000</v>
+      </c>
+      <c r="G20" s="1">
+        <v>76162.356159999996</v>
+      </c>
+      <c r="H20" s="1">
+        <v>109746.63189999999</v>
+      </c>
+      <c r="I20" s="1"/>
+      <c r="L20" t="s">
+        <v>21</v>
+      </c>
+      <c r="M20">
+        <f>B21/1000</f>
+        <v>37.553232429999994</v>
+      </c>
+      <c r="N20">
+        <f t="shared" si="8"/>
+        <v>37.553232429999994</v>
+      </c>
+      <c r="O20">
+        <f t="shared" si="8"/>
+        <v>37.553232429999994</v>
+      </c>
+      <c r="P20">
+        <f t="shared" si="8"/>
+        <v>37.553232429999994</v>
+      </c>
+      <c r="Q20">
+        <f t="shared" si="8"/>
+        <v>37.553232429999994</v>
+      </c>
+      <c r="R20">
+        <f t="shared" si="8"/>
+        <v>38</v>
+      </c>
+      <c r="S20">
+        <f t="shared" si="8"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:19" ht="16">
+      <c r="A21" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B21" s="1">
+        <v>37553.232429999996</v>
+      </c>
+      <c r="C21" s="1">
+        <v>37553.232429999996</v>
+      </c>
+      <c r="D21" s="1">
+        <v>37553.232429999996</v>
+      </c>
+      <c r="E21" s="1">
+        <v>37553.232429999996</v>
+      </c>
+      <c r="F21" s="1">
+        <v>37553.232429999996</v>
+      </c>
+      <c r="G21" s="1">
+        <v>38000</v>
+      </c>
+      <c r="H21" s="1">
+        <v>39000</v>
+      </c>
+      <c r="I21" s="1">
+        <v>40434.007490000004</v>
+      </c>
+    </row>
+    <row r="22" spans="1:19" ht="16">
+      <c r="A22" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B22" s="1">
+        <v>39902.372239999997</v>
+      </c>
+      <c r="C22" s="1">
+        <v>39902.372239999997</v>
+      </c>
+      <c r="D22" s="1">
+        <v>39902.372239999997</v>
+      </c>
+      <c r="E22" s="1">
+        <v>39902.372239999997</v>
+      </c>
+      <c r="F22" s="1">
+        <v>39902.372239999997</v>
+      </c>
+      <c r="G22" s="1">
+        <v>40000</v>
+      </c>
+      <c r="H22" s="1">
+        <v>41000</v>
+      </c>
+      <c r="I22" s="1">
+        <v>40971.968379999998</v>
+      </c>
+    </row>
+    <row r="26" spans="1:19">
+      <c r="D26">
+        <f>D20/D21</f>
+        <v>1.2450044865551939</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="B1" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4">
+        <v>5</v>
+      </c>
+      <c r="C4">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5">
+        <v>8</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <drawing r:id="rId1"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update lorra vs LL to use ASYNC post commit. Added pdf of figs
</commit_message>
<xml_diff>
--- a/figs/results.xlsx
+++ b/figs/results.xlsx
@@ -4,14 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27729"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="3200" yWindow="1480" windowWidth="35200" windowHeight="22060" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="2980" yWindow="2060" windowWidth="25600" windowHeight="16060" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="TXLatency" sheetId="4" r:id="rId4"/>
-    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="27">
   <si>
     <t>Read</t>
   </si>
@@ -70,9 +69,6 @@
     <t>single transaction</t>
   </si>
   <si>
-    <t>omid LL write</t>
-  </si>
-  <si>
     <t>beign</t>
   </si>
   <si>
@@ -85,9 +81,6 @@
     <t>single read</t>
   </si>
   <si>
-    <t>lorra (singletons)</t>
-  </si>
-  <si>
     <t>omid LL</t>
   </si>
   <si>
@@ -95,12 +88,6 @@
   </si>
   <si>
     <t>TX 10</t>
-  </si>
-  <si>
-    <t>lorra (checkAndMutate)</t>
-  </si>
-  <si>
-    <t>omid LL (Put)</t>
   </si>
   <si>
     <t>omid</t>
@@ -115,7 +102,7 @@
     <t>lorra</t>
   </si>
   <si>
-    <t>single write</t>
+    <t xml:space="preserve">lorra </t>
   </si>
 </sst>
 </file>
@@ -123,7 +110,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -196,7 +183,7 @@
     </border>
   </borders>
   <cellStyleXfs count="23">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -221,15 +208,15 @@
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="9">
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="165" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="23">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -461,11 +448,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2110059448"/>
-        <c:axId val="-2110054904"/>
+        <c:axId val="-2036078280"/>
+        <c:axId val="-2036183848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2110059448"/>
+        <c:axId val="-2036078280"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -474,7 +461,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110054904"/>
+        <c:crossAx val="-2036183848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -482,7 +469,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2110054904"/>
+        <c:axId val="-2036183848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -506,21 +493,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2110059448"/>
+        <c:crossAx val="-2036078280"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -565,7 +550,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -777,11 +761,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2077107480"/>
-        <c:axId val="-2077106072"/>
+        <c:axId val="-2137981336"/>
+        <c:axId val="-2035483064"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2077107480"/>
+        <c:axId val="-2137981336"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -803,14 +787,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077106072"/>
+        <c:crossAx val="-2035483064"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -818,7 +801,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077106072"/>
+        <c:axId val="-2035483064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="120.0"/>
@@ -842,21 +825,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077107480"/>
+        <c:crossAx val="-2137981336"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -906,7 +887,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1106,11 +1086,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2077673976"/>
-        <c:axId val="-2077278392"/>
+        <c:axId val="-2035880376"/>
+        <c:axId val="-2035753000"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2077673976"/>
+        <c:axId val="-2035880376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1132,14 +1112,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077278392"/>
+        <c:crossAx val="-2035753000"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1147,7 +1126,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2077278392"/>
+        <c:axId val="-2035753000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1170,21 +1149,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2077673976"/>
+        <c:crossAx val="-2035880376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1234,7 +1211,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -1425,11 +1401,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2061912760"/>
-        <c:axId val="-2061909976"/>
+        <c:axId val="-2036048344"/>
+        <c:axId val="-2035492712"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2061912760"/>
+        <c:axId val="-2036048344"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1451,14 +1427,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061909976"/>
+        <c:crossAx val="-2035492712"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1466,7 +1441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2061909976"/>
+        <c:axId val="-2035492712"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1489,219 +1464,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2061912760"/>
+        <c:crossAx val="-2036048344"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart13.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="118"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="18"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet5!$B$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>lorra</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet5!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>single read</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>single write</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>TX 5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TX 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet5!$B$2:$B$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>7.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>Sheet5!$C$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>omid LL</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:strRef>
-              <c:f>Sheet5!$A$2:$A$5</c:f>
-              <c:strCache>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>single read</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>single write</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>TX 5</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>TX 10</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>Sheet5!$C$2:$C$5</c:f>
-              <c:numCache>
-                <c:formatCode>0.0</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.0</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="-2072820568"/>
-        <c:axId val="-2075784856"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="-2072820568"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2075784856"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="-2075784856"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.0" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2072820568"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -1902,11 +1677,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2109993800"/>
-        <c:axId val="-2109946392"/>
+        <c:axId val="-2036131496"/>
+        <c:axId val="-2036140632"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2109993800"/>
+        <c:axId val="-2036131496"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1915,7 +1690,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109946392"/>
+        <c:crossAx val="-2036140632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1923,7 +1698,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109946392"/>
+        <c:axId val="-2036140632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="8.0"/>
@@ -1947,21 +1722,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109993800"/>
+        <c:crossAx val="-2036131496"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2221,11 +1994,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2109936408"/>
-        <c:axId val="-2109926600"/>
+        <c:axId val="-2035400856"/>
+        <c:axId val="-2035397736"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2109936408"/>
+        <c:axId val="-2035400856"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2234,7 +2007,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109926600"/>
+        <c:crossAx val="-2035397736"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2242,7 +2015,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2109926600"/>
+        <c:axId val="-2035397736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2265,21 +2038,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2109936408"/>
+        <c:crossAx val="-2035400856"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2532,11 +2303,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2131827368"/>
-        <c:axId val="-2131790584"/>
+        <c:axId val="-2055819000"/>
+        <c:axId val="-2055869256"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2131827368"/>
+        <c:axId val="-2055819000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2558,14 +2329,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131790584"/>
+        <c:crossAx val="-2055869256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2574,7 +2344,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2131790584"/>
+        <c:axId val="-2055869256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2597,21 +2367,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2131827368"/>
+        <c:crossAx val="-2055819000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2864,11 +2632,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-2111991624"/>
-        <c:axId val="-2111929880"/>
+        <c:axId val="-2055983640"/>
+        <c:axId val="-2055560040"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-2111991624"/>
+        <c:axId val="-2055983640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2890,14 +2658,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111929880"/>
+        <c:crossAx val="-2055560040"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2905,7 +2672,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111929880"/>
+        <c:axId val="-2055560040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2928,21 +2695,19 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111991624"/>
+        <c:crossAx val="-2055983640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
       <c:legendPos val="r"/>
-      <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
     <c:plotVisOnly val="1"/>
@@ -2978,16 +2743,23 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="0"/>
               <a:t>Single Write</a:t>
             </a:r>
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.33128258967629"/>
+          <c:y val="0.0324074074074074"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
     </c:title>
     <c:autoTitleDeleted val="0"/>
@@ -3018,10 +2790,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL write</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3063,10 +2835,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL write</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3078,10 +2850,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>3.63</c:v>
+                  <c:v>5.31</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.04</c:v>
+                  <c:v>2.95</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3108,10 +2880,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra </c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL write</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3126,7 +2898,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.81</c:v>
+                  <c:v>5.15</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3142,11 +2914,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112840744"/>
-        <c:axId val="-2112502312"/>
+        <c:axId val="-2055727000"/>
+        <c:axId val="-2055731848"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112840744"/>
+        <c:axId val="-2055727000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3155,7 +2927,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112502312"/>
+        <c:crossAx val="-2055731848"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3163,7 +2935,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2112502312"/>
+        <c:axId val="-2055731848"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3177,10 +2949,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" b="0"/>
                   <a:t>[msec]</a:t>
                 </a:r>
               </a:p>
@@ -3193,7 +2965,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112840744"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055727000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3246,10 +3028,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="0"/>
               <a:t>Single Read</a:t>
             </a:r>
           </a:p>
@@ -3286,7 +3068,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>omid LL</c:v>
@@ -3304,7 +3086,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.27</c:v>
+                  <c:v>0.26</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3331,7 +3113,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>omid LL</c:v>
@@ -3346,10 +3128,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>1.51</c:v>
+                  <c:v>2.2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1.66</c:v>
+                  <c:v>2.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3376,7 +3158,7 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (singletons)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>omid LL</c:v>
@@ -3394,7 +3176,7 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.0</c:v>
+                  <c:v>0.25</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3410,11 +3192,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2080155560"/>
-        <c:axId val="-2111993896"/>
+        <c:axId val="-2055556104"/>
+        <c:axId val="-2055553384"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2080155560"/>
+        <c:axId val="-2055556104"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3423,7 +3205,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2111993896"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055553384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3431,10 +3223,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2111993896"/>
+        <c:axId val="-2055553384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="10.0"/>
+          <c:max val="4.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3446,23 +3238,40 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" b="0"/>
                   <a:t>[msec]</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.0472222222222222"/>
+              <c:y val="0.405752964174142"/>
+            </c:manualLayout>
+          </c:layout>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0.0" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080155560"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055556104"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3505,17 +3314,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="0"/>
               <a:t>TX Size</a:t>
             </a:r>
             <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
+              <a:rPr lang="en-US" sz="2000" b="0" baseline="0"/>
               <a:t> 5</a:t>
             </a:r>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="en-US" sz="2000" b="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -3550,10 +3359,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3565,7 +3374,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>0.28</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.29</c:v>
@@ -3595,10 +3404,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3610,10 +3419,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>13.57</c:v>
+                  <c:v>20.08</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>8.79</c:v>
+                  <c:v>12.33</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3640,10 +3449,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3655,10 +3464,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12.85</c:v>
+                  <c:v>5.72</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>12.06</c:v>
+                  <c:v>5.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3674,11 +3483,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2080025416"/>
-        <c:axId val="-2128165112"/>
+        <c:axId val="-2055500264"/>
+        <c:axId val="-2055497256"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2080025416"/>
+        <c:axId val="-2055500264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3687,7 +3496,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2128165112"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055497256"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3695,10 +3514,10 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2128165112"/>
+        <c:axId val="-2055497256"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="60.0"/>
+          <c:max val="30.0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3710,10 +3529,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr sz="2000" b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" sz="2000" b="0"/>
                   <a:t>[msec]</a:t>
                 </a:r>
               </a:p>
@@ -3726,7 +3545,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2080025416"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055500264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3769,10 +3598,10 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr/>
+              <a:defRPr sz="2000" b="0"/>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-US"/>
+              <a:rPr lang="en-US" sz="2000" b="0"/>
               <a:t>TX Size 10</a:t>
             </a:r>
           </a:p>
@@ -3809,10 +3638,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3824,7 +3653,7 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>0.33</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.29</c:v>
@@ -3854,10 +3683,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3869,10 +3698,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>27.14</c:v>
+                  <c:v>40.15</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>17.57</c:v>
+                  <c:v>24.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3899,10 +3728,10 @@
               <c:strCache>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>lorra (checkAndMutate)</c:v>
+                  <c:v>lorra</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>omid LL (Put)</c:v>
+                  <c:v>omid LL</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3914,10 +3743,10 @@
                 <c:formatCode>0.0</c:formatCode>
                 <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>23.68</c:v>
+                  <c:v>4.02</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>22.86</c:v>
+                  <c:v>5.53</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3933,11 +3762,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="-2112594856"/>
-        <c:axId val="-2126249720"/>
+        <c:axId val="-2055459448"/>
+        <c:axId val="-2055456472"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="-2112594856"/>
+        <c:axId val="-2055459448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3946,7 +3775,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2126249720"/>
+        <c:crossAx val="-2055456472"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3954,7 +3783,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-2126249720"/>
+        <c:axId val="-2055456472"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3968,10 +3797,10 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr/>
+                  <a:defRPr b="0"/>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-US"/>
+                  <a:rPr lang="en-US" b="0"/>
                   <a:t>[msec]</a:t>
                 </a:r>
               </a:p>
@@ -3984,7 +3813,17 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="-2112594856"/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600"/>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2055459448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4180,16 +4019,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>800100</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>20</xdr:col>
-      <xdr:colOff>596900</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>196850</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4219,7 +4058,7 @@
       <xdr:col>12</xdr:col>
       <xdr:colOff>749300</xdr:colOff>
       <xdr:row>14</xdr:row>
-      <xdr:rowOff>82550</xdr:rowOff>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4240,16 +4079,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>317500</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>774700</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>184150</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>762000</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>393700</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4271,15 +4110,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>419100</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:colOff>25400</xdr:colOff>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>21</xdr:col>
-      <xdr:colOff>215900</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>165100</xdr:rowOff>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -4388,41 +4227,6 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>11</xdr:col>
-      <xdr:colOff>622300</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>101600</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>241300</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>177800</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -5627,8 +5431,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M38" sqref="M38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5646,15 +5450,15 @@
     <row r="2" spans="1:3" ht="16">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="16">
       <c r="A3" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B3" s="1">
         <v>0</v>
@@ -5665,24 +5469,24 @@
     </row>
     <row r="4" spans="1:3" ht="16">
       <c r="A4" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B4" s="1">
-        <v>3.63</v>
+        <v>5.31</v>
       </c>
       <c r="C4" s="1">
-        <v>2.04</v>
+        <v>2.95</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="16">
       <c r="A5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B5" s="1">
         <v>0</v>
       </c>
       <c r="C5" s="1">
-        <v>6.81</v>
+        <v>5.15</v>
       </c>
     </row>
     <row r="6" spans="1:3" ht="16">
@@ -5702,7 +5506,7 @@
     </row>
     <row r="9" spans="1:3" ht="16">
       <c r="A9" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -5710,43 +5514,43 @@
     <row r="10" spans="1:3" ht="16">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="11" spans="1:3" ht="16">
       <c r="A11" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B11" s="1">
         <v>0</v>
       </c>
       <c r="C11" s="1">
-        <v>0.27</v>
+        <v>0.26</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="16">
       <c r="A12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B12" s="1">
-        <v>1.51</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="C12" s="1">
-        <v>1.66</v>
+        <v>2.33</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="16">
       <c r="A13" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
       </c>
       <c r="C13" s="1">
-        <v>0</v>
+        <v>0.25</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="16">
@@ -5779,18 +5583,18 @@
     <row r="19" spans="1:3" ht="16">
       <c r="A19" s="1"/>
       <c r="B19" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="16">
       <c r="A20" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>0.33</v>
+        <v>0.28000000000000003</v>
       </c>
       <c r="C20" s="1">
         <v>0.28999999999999998</v>
@@ -5798,24 +5602,24 @@
     </row>
     <row r="21" spans="1:3" ht="16">
       <c r="A21" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B21" s="1">
-        <v>13.57</v>
+        <v>20.079999999999998</v>
       </c>
       <c r="C21" s="1">
-        <v>8.7899999999999991</v>
+        <v>12.33</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="16">
       <c r="A22" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B22" s="1">
-        <v>12.85</v>
+        <v>5.72</v>
       </c>
       <c r="C22" s="1">
-        <v>12.06</v>
+        <v>5.2</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="16">
@@ -5830,7 +5634,7 @@
     </row>
     <row r="25" spans="1:3" ht="16">
       <c r="A25" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -5838,18 +5642,18 @@
     <row r="26" spans="1:3" ht="16">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C26" s="1" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="17">
       <c r="A27" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B27" s="8">
-        <v>0.33</v>
+        <v>0</v>
       </c>
       <c r="C27" s="8">
         <v>0.28999999999999998</v>
@@ -5857,24 +5661,24 @@
     </row>
     <row r="28" spans="1:3" ht="17">
       <c r="A28" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B28" s="8">
-        <v>27.14</v>
+        <v>40.15</v>
       </c>
       <c r="C28" s="8">
-        <v>17.57</v>
+        <v>24.67</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="16">
       <c r="A29" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B29" s="1">
-        <v>23.68</v>
+        <v>4.0199999999999996</v>
       </c>
       <c r="C29" s="1">
-        <v>22.86</v>
+        <v>5.53</v>
       </c>
     </row>
   </sheetData>
@@ -5950,41 +5754,41 @@
         <v>35.886000000000003</v>
       </c>
       <c r="N2">
-        <f>D2/1000</f>
+        <f t="shared" ref="N2:U2" si="0">D2/1000</f>
         <v>63.908999999999999</v>
       </c>
       <c r="O2">
-        <f>E2/1000</f>
+        <f t="shared" si="0"/>
         <v>108.821</v>
       </c>
       <c r="P2">
-        <f>F2/1000</f>
+        <f t="shared" si="0"/>
         <v>115.373</v>
       </c>
       <c r="Q2">
-        <f>G2/1000</f>
+        <f t="shared" si="0"/>
         <v>165.48699999999999</v>
       </c>
       <c r="R2">
-        <f>H2/1000</f>
+        <f t="shared" si="0"/>
         <v>269.89100000000002</v>
       </c>
       <c r="S2">
-        <f>I2/1000</f>
+        <f t="shared" si="0"/>
         <v>288.53699999999998</v>
       </c>
       <c r="T2">
-        <f>J2/1000</f>
+        <f t="shared" si="0"/>
         <v>301.25799999999998</v>
       </c>
       <c r="U2">
-        <f>K2/1000</f>
+        <f t="shared" si="0"/>
         <v>360.33699999999999</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="16">
       <c r="A3" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B3" s="1">
         <v>18754.96056</v>
@@ -6015,44 +5819,44 @@
       </c>
       <c r="K3" s="1"/>
       <c r="L3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M3">
         <f>B3/1000</f>
         <v>18.754960560000001</v>
       </c>
       <c r="N3">
-        <f>D3/1000</f>
+        <f t="shared" ref="N3:T4" si="1">D3/1000</f>
         <v>20.357945579999999</v>
       </c>
       <c r="O3">
-        <f>E3/1000</f>
+        <f t="shared" si="1"/>
         <v>22.128590370000001</v>
       </c>
       <c r="P3">
-        <f>F3/1000</f>
+        <f t="shared" si="1"/>
         <v>23</v>
       </c>
       <c r="Q3">
-        <f>G3/1000</f>
+        <f t="shared" si="1"/>
         <v>32.656683770000001</v>
       </c>
       <c r="R3">
-        <f>H3/1000</f>
+        <f t="shared" si="1"/>
         <v>45.784195509999996</v>
       </c>
       <c r="S3">
-        <f>I3/1000</f>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="T3">
-        <f>J3/1000</f>
+        <f t="shared" si="1"/>
         <v>73.094409639999995</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="16">
       <c r="A4" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B4" s="1">
         <v>5800</v>
@@ -6085,38 +5889,38 @@
         <v>8955.5921500000004</v>
       </c>
       <c r="L4" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M4">
         <f>B4/1000</f>
         <v>5.8</v>
       </c>
       <c r="N4">
-        <f>D4/1000</f>
+        <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
       <c r="O4">
-        <f>E4/1000</f>
+        <f t="shared" si="1"/>
         <v>5.9</v>
       </c>
       <c r="P4">
-        <f>F4/1000</f>
+        <f t="shared" si="1"/>
         <v>5.9080332750000002</v>
       </c>
       <c r="Q4">
-        <f>G4/1000</f>
+        <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
       <c r="R4">
-        <f>H4/1000</f>
+        <f t="shared" si="1"/>
         <v>4.9000000000000004</v>
       </c>
       <c r="S4">
-        <f>I4/1000</f>
+        <f t="shared" si="1"/>
         <v>4.9877389469999995</v>
       </c>
       <c r="T4">
-        <f>J4/1000</f>
+        <f t="shared" si="1"/>
         <v>6</v>
       </c>
       <c r="U4">
@@ -6126,7 +5930,7 @@
     </row>
     <row r="5" spans="1:21" ht="16">
       <c r="A5" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B5" s="1">
         <v>6800</v>
@@ -6193,37 +5997,37 @@
         <v>35.886000000000003</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:T10" si="0">C10/1000</f>
+        <f t="shared" ref="N10:T10" si="2">C10/1000</f>
         <v>63.908999999999999</v>
       </c>
       <c r="O10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>108.821</v>
       </c>
       <c r="P10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>165.48699999999999</v>
       </c>
       <c r="Q10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>256.92500000000001</v>
       </c>
       <c r="R10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>269.89100000000002</v>
       </c>
       <c r="S10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>301.25799999999998</v>
       </c>
       <c r="T10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="2"/>
         <v>360.33699999999999</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="16">
       <c r="A11" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B11" s="1">
         <v>32008</v>
@@ -6248,40 +6052,40 @@
       </c>
       <c r="I11" s="1"/>
       <c r="L11" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M11">
-        <f t="shared" ref="M11:M12" si="1">B11/1000</f>
+        <f t="shared" ref="M11:M12" si="3">B11/1000</f>
         <v>32.008000000000003</v>
       </c>
       <c r="N11">
-        <f t="shared" ref="N11:N12" si="2">C11/1000</f>
+        <f t="shared" ref="N11:N12" si="4">C11/1000</f>
         <v>33.266133329999995</v>
       </c>
       <c r="O11">
-        <f t="shared" ref="O11:O12" si="3">D11/1000</f>
+        <f t="shared" ref="O11:O12" si="5">D11/1000</f>
         <v>37.403168669999999</v>
       </c>
       <c r="P11">
-        <f t="shared" ref="P11:P12" si="4">E11/1000</f>
+        <f t="shared" ref="P11:P12" si="6">E11/1000</f>
         <v>47.177634850000004</v>
       </c>
       <c r="Q11">
-        <f t="shared" ref="Q11:Q12" si="5">F11/1000</f>
+        <f t="shared" ref="Q11:Q12" si="7">F11/1000</f>
         <v>63</v>
       </c>
       <c r="R11">
-        <f t="shared" ref="R11:R12" si="6">G11/1000</f>
+        <f t="shared" ref="R11:R12" si="8">G11/1000</f>
         <v>67.3873265</v>
       </c>
       <c r="S11">
-        <f t="shared" ref="S11:T12" si="7">H11/1000</f>
+        <f t="shared" ref="S11:T12" si="9">H11/1000</f>
         <v>100.8789393</v>
       </c>
     </row>
     <row r="12" spans="1:21" ht="16">
       <c r="A12" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B12" s="1">
         <v>18414.79408</v>
@@ -6308,44 +6112,44 @@
         <v>23023.44454</v>
       </c>
       <c r="L12" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M12">
-        <f t="shared" si="1"/>
-        <v>18.41479408</v>
-      </c>
-      <c r="N12">
-        <f t="shared" si="2"/>
-        <v>18.41479408</v>
-      </c>
-      <c r="O12">
         <f t="shared" si="3"/>
         <v>18.41479408</v>
       </c>
-      <c r="P12">
+      <c r="N12">
         <f t="shared" si="4"/>
         <v>18.41479408</v>
       </c>
-      <c r="Q12">
+      <c r="O12">
         <f t="shared" si="5"/>
         <v>18.41479408</v>
       </c>
+      <c r="P12">
+        <f t="shared" si="6"/>
+        <v>18.41479408</v>
+      </c>
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>18.41479408</v>
+      </c>
       <c r="R12">
-        <f t="shared" si="6"/>
+        <f t="shared" si="8"/>
         <v>20</v>
       </c>
       <c r="S12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>23</v>
       </c>
       <c r="T12">
-        <f t="shared" si="7"/>
+        <f t="shared" si="9"/>
         <v>23.02344454</v>
       </c>
     </row>
     <row r="13" spans="1:21" ht="16">
       <c r="A13" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B13" s="1">
         <v>19528.699280000001</v>
@@ -6374,7 +6178,7 @@
     </row>
     <row r="18" spans="1:19" ht="16">
       <c r="A18" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -6385,31 +6189,31 @@
       <c r="H18" s="1"/>
       <c r="I18" s="1"/>
       <c r="M18">
-        <f>B19/1000</f>
+        <f t="shared" ref="M18:S18" si="10">B19/1000</f>
         <v>35.886000000000003</v>
       </c>
       <c r="N18">
-        <f>C19/1000</f>
+        <f t="shared" si="10"/>
         <v>63.908999999999999</v>
       </c>
       <c r="O18">
-        <f>D19/1000</f>
+        <f t="shared" si="10"/>
         <v>108.821</v>
       </c>
       <c r="P18">
-        <f>E19/1000</f>
+        <f t="shared" si="10"/>
         <v>165.48699999999999</v>
       </c>
       <c r="Q18">
-        <f>F19/1000</f>
+        <f t="shared" si="10"/>
         <v>256.92500000000001</v>
       </c>
       <c r="R18">
-        <f>G19/1000</f>
+        <f t="shared" si="10"/>
         <v>269.89100000000002</v>
       </c>
       <c r="S18">
-        <f>H19/1000</f>
+        <f t="shared" si="10"/>
         <v>301.25799999999998</v>
       </c>
     </row>
@@ -6440,40 +6244,40 @@
         <v>360337</v>
       </c>
       <c r="L19" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="M19">
         <f>B20/1000</f>
         <v>41.087000000000003</v>
       </c>
       <c r="N19">
-        <f t="shared" ref="N19:S20" si="8">C20/1000</f>
+        <f t="shared" ref="N19:S20" si="11">C20/1000</f>
         <v>44.390378380000001</v>
       </c>
       <c r="O19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>46.753942860000002</v>
       </c>
       <c r="P19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>57.097809950000006</v>
       </c>
       <c r="Q19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>70</v>
       </c>
       <c r="R19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>76.162356160000002</v>
       </c>
       <c r="S19">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>109.7466319</v>
       </c>
     </row>
     <row r="20" spans="1:19" ht="16">
       <c r="A20" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B20" s="1">
         <v>41087</v>
@@ -6498,40 +6302,40 @@
       </c>
       <c r="I20" s="1"/>
       <c r="L20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="M20">
         <f>B21/1000</f>
         <v>37.553232429999994</v>
       </c>
       <c r="N20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>37.553232429999994</v>
       </c>
       <c r="O20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>37.553232429999994</v>
       </c>
       <c r="P20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>37.553232429999994</v>
       </c>
       <c r="Q20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>37.553232429999994</v>
       </c>
       <c r="R20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>38</v>
       </c>
       <c r="S20">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="1:19" ht="16">
       <c r="A21" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B21" s="1">
         <v>37553.232429999996</v>
@@ -6560,7 +6364,7 @@
     </row>
     <row r="22" spans="1:19" ht="16">
       <c r="A22" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B22" s="1">
         <v>39902.372239999997</v>
@@ -6603,77 +6407,4 @@
     </ext>
   </extLst>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData>
-    <row r="1" spans="1:3">
-      <c r="B1" t="s">
-        <v>29</v>
-      </c>
-      <c r="C1" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
-        <v>19</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
-      <c r="A3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B3">
-        <v>3</v>
-      </c>
-      <c r="C3">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
-      <c r="A4" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4">
-        <v>5</v>
-      </c>
-      <c r="C4">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
-      <c r="A5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B5">
-        <v>7</v>
-      </c>
-      <c r="C5">
-        <v>8</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <drawing r:id="rId1"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
-</worksheet>
 </file>
</xml_diff>